<commit_message>
Using the 128 version to collect similarity (Old/Similar/New) Response
Will change it back later
- Also changed a few sounds to increase similarity
</commit_message>
<xml_diff>
--- a/Analysis/Similarity_analysis.xlsx
+++ b/Analysis/Similarity_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{05B3CA01-97AE-4C07-9B70-1C44C383DEA3}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C87C2E77-A0E6-4E4A-9D5B-4065D245E346}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1154,8 +1154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1164,240 +1164,244 @@
     <col min="2" max="2" width="17.36328125" customWidth="1"/>
     <col min="3" max="3" width="17.90625" customWidth="1"/>
     <col min="4" max="4" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="16.90625" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" customWidth="1"/>
+    <col min="12" max="12" width="21.08984375" customWidth="1"/>
     <col min="22" max="22" width="16.7265625" customWidth="1"/>
     <col min="23" max="23" width="20.81640625" customWidth="1"/>
     <col min="24" max="24" width="18.7265625" customWidth="1"/>
     <col min="25" max="25" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>23</v>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="8"/>
+    </row>
+    <row r="2" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="Y2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>13</v>
+        <v>87</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
       <c r="K3" s="2">
@@ -1410,18 +1414,18 @@
         <v>2</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O3">
         <v>3</v>
       </c>
-      <c r="P3" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>3</v>
-      </c>
-      <c r="R3" s="2">
+      <c r="P3">
+        <v>2</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
         <v>3</v>
       </c>
       <c r="S3">
@@ -1430,76 +1434,77 @@
       <c r="T3">
         <v>3</v>
       </c>
-      <c r="U3">
-        <v>3</v>
+      <c r="U3" s="3">
+        <v>2</v>
       </c>
       <c r="V3">
         <v>2</v>
       </c>
-      <c r="W3">
-        <v>3</v>
-      </c>
-      <c r="X3" s="2">
+      <c r="X3">
         <v>3</v>
       </c>
       <c r="Y3">
         <v>3</v>
       </c>
-      <c r="Z3">
-        <v>2</v>
-      </c>
-      <c r="AA3">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>3</v>
+      <c r="Z3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB3">
+        <v>2</v>
       </c>
       <c r="AD3">
         <v>2</v>
       </c>
       <c r="AE3">
-        <v>3</v>
-      </c>
-      <c r="AH3">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI3">
+        <v>1</v>
+      </c>
+      <c r="AJ3" s="3"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="3">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
       <c r="K4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -1510,14 +1515,14 @@
       <c r="O4">
         <v>1</v>
       </c>
-      <c r="P4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2">
-        <v>2</v>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
       </c>
       <c r="S4">
         <v>1</v>
@@ -1525,32 +1530,26 @@
       <c r="T4">
         <v>1</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="3">
         <v>1</v>
       </c>
       <c r="V4">
         <v>1</v>
       </c>
-      <c r="W4">
-        <v>1</v>
-      </c>
-      <c r="X4" s="2">
+      <c r="X4">
         <v>1</v>
       </c>
       <c r="Y4">
         <v>1</v>
       </c>
-      <c r="Z4">
-        <v>1</v>
-      </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>2</v>
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>1</v>
       </c>
       <c r="AD4">
         <v>2</v>
@@ -1558,57 +1557,64 @@
       <c r="AE4">
         <v>2</v>
       </c>
-      <c r="AH4">
-        <v>2</v>
-      </c>
+      <c r="AG4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI4">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="3"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="3">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="3">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
       </c>
       <c r="K5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5">
         <v>2</v>
       </c>
       <c r="M5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>2</v>
       </c>
       <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>3</v>
-      </c>
-      <c r="R5" s="2">
+        <v>3</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
         <v>2</v>
       </c>
       <c r="S5">
@@ -1617,8 +1623,8 @@
       <c r="T5">
         <v>2</v>
       </c>
-      <c r="U5">
-        <v>2</v>
+      <c r="U5" s="3">
+        <v>3</v>
       </c>
       <c r="V5">
         <v>2</v>
@@ -1626,60 +1632,61 @@
       <c r="W5">
         <v>3</v>
       </c>
-      <c r="X5" s="2">
+      <c r="X5">
         <v>2</v>
       </c>
       <c r="Y5">
         <v>2</v>
       </c>
-      <c r="Z5">
-        <v>2</v>
-      </c>
-      <c r="AA5">
-        <v>2</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD5">
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5">
         <v>2</v>
       </c>
       <c r="AE5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF5">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH5" s="3">
+        <v>2</v>
       </c>
       <c r="AI5">
         <v>2</v>
       </c>
+      <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3">
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="I6" s="2">
+        <v>2</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
       <c r="K6" s="2">
@@ -1697,13 +1704,13 @@
       <c r="O6">
         <v>2</v>
       </c>
-      <c r="P6" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>3</v>
-      </c>
-      <c r="R6" s="2">
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
         <v>2</v>
       </c>
       <c r="S6">
@@ -1712,7 +1719,7 @@
       <c r="T6">
         <v>2</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="3">
         <v>2</v>
       </c>
       <c r="V6">
@@ -1721,25 +1728,19 @@
       <c r="W6">
         <v>2</v>
       </c>
-      <c r="X6" s="2">
-        <v>3</v>
+      <c r="X6">
+        <v>2</v>
       </c>
       <c r="Y6">
         <v>2</v>
       </c>
-      <c r="Z6">
-        <v>2</v>
-      </c>
-      <c r="AA6">
-        <v>2</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC6" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD6">
+      <c r="Z6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB6">
         <v>2</v>
       </c>
       <c r="AE6">
@@ -1748,114 +1749,122 @@
       <c r="AF6">
         <v>2</v>
       </c>
+      <c r="AG6" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH6" s="3">
+        <v>1</v>
+      </c>
       <c r="AI6">
         <v>2</v>
       </c>
+      <c r="AJ6" s="3"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="3">
-        <v>3</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7" s="3">
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>3</v>
+      </c>
+      <c r="J7">
         <v>2</v>
       </c>
       <c r="K7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7">
         <v>2</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O7">
         <v>2</v>
       </c>
-      <c r="P7" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>3</v>
-      </c>
-      <c r="R7" s="2">
-        <v>2</v>
+      <c r="P7">
+        <v>2</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
       </c>
       <c r="S7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T7">
         <v>2</v>
       </c>
-      <c r="U7">
-        <v>2</v>
+      <c r="U7" s="3">
+        <v>3</v>
       </c>
       <c r="V7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W7">
         <v>2</v>
       </c>
-      <c r="X7" s="2">
-        <v>3</v>
+      <c r="X7">
+        <v>2</v>
       </c>
       <c r="Y7">
         <v>2</v>
       </c>
-      <c r="Z7">
-        <v>2</v>
-      </c>
-      <c r="AA7">
-        <v>2</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC7" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD7">
+      <c r="Z7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB7">
         <v>2</v>
       </c>
       <c r="AE7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AF7">
         <v>2</v>
       </c>
+      <c r="AG7" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH7" s="3">
+        <v>2</v>
+      </c>
       <c r="AI7">
         <v>2</v>
       </c>
+      <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
       <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1867,13 +1876,13 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -1882,7 +1891,7 @@
         <v>2</v>
       </c>
       <c r="M8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>2</v>
@@ -1897,7 +1906,7 @@
         <v>2</v>
       </c>
       <c r="R8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8">
         <v>2</v>
@@ -1906,7 +1915,7 @@
         <v>2</v>
       </c>
       <c r="U8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V8">
         <v>2</v>
@@ -1932,11 +1941,8 @@
       <c r="AC8">
         <v>2</v>
       </c>
-      <c r="AD8">
-        <v>2</v>
-      </c>
       <c r="AE8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF8">
         <v>2</v>
@@ -1947,19 +1953,22 @@
       <c r="AI8">
         <v>2</v>
       </c>
+      <c r="AJ8">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
       <c r="E9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1974,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="J9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1986,7 +1995,7 @@
         <v>3</v>
       </c>
       <c r="N9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O9">
         <v>2</v>
@@ -1995,7 +2004,7 @@
         <v>3</v>
       </c>
       <c r="Q9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R9">
         <v>2</v>
@@ -2010,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="V9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W9">
         <v>2</v>
@@ -2022,20 +2031,17 @@
         <v>2</v>
       </c>
       <c r="Z9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AA9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AC9">
         <v>2</v>
       </c>
-      <c r="AD9">
-        <v>3</v>
-      </c>
       <c r="AE9">
         <v>2</v>
       </c>
@@ -2048,28 +2054,31 @@
       <c r="AI9">
         <v>2</v>
       </c>
+      <c r="AJ9">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
       <c r="C10">
         <v>1</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
       <c r="E10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <v>2</v>
@@ -2081,13 +2090,13 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O10">
         <v>2</v>
@@ -2096,10 +2105,10 @@
         <v>2</v>
       </c>
       <c r="Q10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S10">
         <v>2</v>
@@ -2108,16 +2117,16 @@
         <v>2</v>
       </c>
       <c r="U10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W10">
         <v>2</v>
       </c>
       <c r="X10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Y10">
         <v>2</v>
@@ -2134,11 +2143,8 @@
       <c r="AC10">
         <v>2</v>
       </c>
-      <c r="AD10">
-        <v>3</v>
-      </c>
       <c r="AE10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF10">
         <v>2</v>
@@ -2147,44 +2153,48 @@
         <v>2</v>
       </c>
       <c r="AI10">
+        <v>1</v>
+      </c>
+      <c r="AJ10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="3">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="I11" s="3">
-        <v>1</v>
+      <c r="B11" s="2">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>2</v>
       </c>
       <c r="K11" s="2">
-        <v>2</v>
-      </c>
-      <c r="L11">
-        <v>3</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11">
-        <v>2</v>
-      </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="P11" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>3</v>
-      </c>
-      <c r="R11" s="2">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
       </c>
       <c r="S11">
         <v>2</v>
@@ -2192,226 +2202,229 @@
       <c r="T11">
         <v>2</v>
       </c>
-      <c r="U11">
-        <v>2</v>
-      </c>
-      <c r="X11" s="2">
-        <v>3</v>
+      <c r="U11" s="3">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>2</v>
+      </c>
+      <c r="X11">
+        <v>2</v>
       </c>
       <c r="Y11">
         <v>2</v>
       </c>
-      <c r="Z11">
-        <v>2</v>
-      </c>
-      <c r="AA11">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC11" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD11">
-        <v>2</v>
-      </c>
+      <c r="Z11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AG11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AJ11" s="3"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>2</v>
       </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="I12" s="3">
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2">
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="I12" s="2">
+        <v>3</v>
+      </c>
+      <c r="J12">
         <v>3</v>
       </c>
       <c r="K12" s="2">
         <v>3</v>
       </c>
-      <c r="L12">
-        <v>3</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12">
-        <v>3</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12" s="3">
-        <v>2</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>3</v>
-      </c>
-      <c r="R12" s="2">
-        <v>3</v>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
       </c>
       <c r="S12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T12">
         <v>3</v>
       </c>
-      <c r="U12">
-        <v>2</v>
-      </c>
-      <c r="X12" s="2">
+      <c r="U12" s="3">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>3</v>
+      </c>
+      <c r="X12">
         <v>2</v>
       </c>
       <c r="Y12">
-        <v>3</v>
-      </c>
-      <c r="Z12">
-        <v>3</v>
-      </c>
-      <c r="AA12">
-        <v>2</v>
-      </c>
-      <c r="AB12" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC12" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD12">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB12">
+        <v>2</v>
+      </c>
+      <c r="AG12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AJ12" s="3"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>3</v>
       </c>
-      <c r="D13" s="3">
-        <v>1</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="I13" s="3">
-        <v>1</v>
+      <c r="B13" s="2">
+        <v>2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>2</v>
       </c>
       <c r="K13" s="2">
-        <v>3</v>
-      </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-      <c r="N13">
-        <v>2</v>
-      </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-      <c r="P13" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>2</v>
-      </c>
-      <c r="R13" s="2">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
       </c>
       <c r="S13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
-      <c r="U13">
-        <v>2</v>
-      </c>
-      <c r="X13" s="2">
+      <c r="U13" s="3">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="X13">
         <v>2</v>
       </c>
       <c r="Y13">
-        <v>2</v>
-      </c>
-      <c r="Z13">
-        <v>2</v>
-      </c>
-      <c r="AA13">
-        <v>2</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC13" s="2">
-        <v>2</v>
-      </c>
-      <c r="AD13">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB13">
+        <v>2</v>
+      </c>
+      <c r="AG13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AJ13" s="3"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="I14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-      <c r="X14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
+      <c r="U14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AJ14" s="3"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <f>COUNTIF(B3:B13,1)</f>
-        <v>1</v>
-      </c>
-      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="C15" s="2">
         <f>COUNTIF(C3:C13,1)</f>
-        <v>4</v>
-      </c>
-      <c r="D15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15">
         <f>COUNTIF(D3:D13,1)</f>
-        <v>5</v>
-      </c>
-      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
         <f>COUNTIF(E3:E13,1)</f>
         <v>3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <f>COUNTIF(F3:F13,1)</f>
-        <v>3</v>
-      </c>
-      <c r="G15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15">
         <f>COUNTIF(G3:G13,1)</f>
         <v>3</v>
       </c>
       <c r="H15">
         <f>COUNTIF(H3:H13,1)</f>
-        <v>3</v>
-      </c>
-      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2">
         <f>COUNTIF(I3:I13,1)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <f>COUNTIF(J3:J13,1)</f>
-        <v>1</v>
-      </c>
-      <c r="K15" s="9">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
         <f>COUNTIF(K3:K13,1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <f>COUNTIF(L3:L13,1)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <f>COUNTIF(M3:M13,1)</f>
@@ -2419,65 +2432,65 @@
       </c>
       <c r="N15">
         <f>COUNTIF(N3:N13,1)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O15">
         <f>COUNTIF(O3:O13,1)</f>
-        <v>3</v>
-      </c>
-      <c r="P15" s="3">
+        <v>1</v>
+      </c>
+      <c r="P15">
         <f>COUNTIF(P3:P13,1)</f>
         <v>3</v>
       </c>
-      <c r="Q15" s="2">
+      <c r="Q15">
         <f>COUNTIF(Q3:Q13,1)</f>
-        <v>2</v>
-      </c>
-      <c r="R15" s="2">
+        <v>3</v>
+      </c>
+      <c r="R15">
         <f>COUNTIF(R3:R13,1)</f>
         <v>2</v>
       </c>
       <c r="S15">
         <f>COUNTIF(S3:S13,1)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T15">
         <f>COUNTIF(T3:T13,1)</f>
         <v>2</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="3">
         <f>COUNTIF(U3:U13,1)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V15">
         <f>COUNTIF(V3:V13,1)</f>
         <v>1</v>
       </c>
-      <c r="W15">
+      <c r="W15" s="9">
         <f>COUNTIF(W3:W13,1)</f>
-        <v>1</v>
-      </c>
-      <c r="X15" s="2">
+        <v>0</v>
+      </c>
+      <c r="X15">
         <f>COUNTIF(X3:X13,1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y15">
         <f>COUNTIF(Y3:Y13,1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Z15">
         <f>COUNTIF(Z3:Z13,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AA15">
+        <v>4</v>
+      </c>
+      <c r="AA15" s="3">
         <f>COUNTIF(AA3:AA13,1)</f>
-        <v>1</v>
-      </c>
-      <c r="AB15" s="2">
+        <v>3</v>
+      </c>
+      <c r="AB15">
         <f>COUNTIF(AB3:AB13,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AC15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC15">
         <f>COUNTIF(AC3:AC13,1)</f>
         <v>0</v>
       </c>
@@ -2487,82 +2500,86 @@
       </c>
       <c r="AE15">
         <f>COUNTIF(AE3:AE13,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AF15" s="9">
+        <v>4</v>
+      </c>
+      <c r="AF15">
         <f>COUNTIF(AF3:AF13,1)</f>
         <v>0</v>
       </c>
-      <c r="AG15">
+      <c r="AG15" s="3">
         <f>COUNTIF(AG3:AG13,1)</f>
-        <v>0</v>
-      </c>
-      <c r="AH15">
+        <v>3</v>
+      </c>
+      <c r="AH15" s="3">
         <f>COUNTIF(AH3:AH13,1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AI15">
         <f>COUNTIF(AI3:AI13,1)</f>
+        <v>3</v>
+      </c>
+      <c r="AJ15" s="3">
+        <f>COUNTIF(AJ3:AJ13,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:36" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="B16" s="5">
-        <f>B15/2</f>
+        <f>B15/11</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="5">
+        <f>C15/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="D16" s="5">
+        <f>D15/2</f>
         <v>0.5</v>
       </c>
-      <c r="C16" s="5">
-        <f>C15/8</f>
-        <v>0.5</v>
-      </c>
-      <c r="D16" s="5">
-        <f>D15/11</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="E16" s="5">
-        <f>E15/8</f>
+      <c r="E16" s="10">
+        <f>E15/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F16" s="5">
+        <f>F15/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="G16" s="5">
+        <f>G15/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="H16" s="5">
+        <f>H15/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I16" s="5">
+        <f>I15/11</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <f>J15/11</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <f>K15/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="L16" s="5">
+        <f>L15/8</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <f>M15/8</f>
         <v>0.375</v>
       </c>
-      <c r="F16" s="5">
-        <f>F15/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="G16" s="5">
-        <f>G15/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="H16" s="5">
-        <f>H15/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="I16" s="10">
-        <f>I15/11</f>
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="J16" s="5">
-        <f>J15/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K16" s="10">
-        <f>K15/11</f>
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="L16" s="5">
-        <f>L15/11</f>
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="M16" s="5">
-        <f>M15/11</f>
-        <v>0.27272727272727271</v>
-      </c>
       <c r="N16" s="5">
-        <f>N15/11</f>
-        <v>0.27272727272727271</v>
+        <f>N15/8</f>
+        <v>0.125</v>
       </c>
       <c r="O16" s="5">
-        <f>O15/11</f>
-        <v>0.27272727272727271</v>
+        <f>O15/8</f>
+        <v>0.125</v>
       </c>
       <c r="P16" s="5">
         <f>P15/11</f>
@@ -2570,7 +2587,7 @@
       </c>
       <c r="Q16" s="5">
         <f>Q15/11</f>
-        <v>0.18181818181818182</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="R16" s="5">
         <f>R15/11</f>
@@ -2578,7 +2595,7 @@
       </c>
       <c r="S16" s="5">
         <f>S15/11</f>
-        <v>0.18181818181818182</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="T16" s="5">
         <f>T15/11</f>
@@ -2586,62 +2603,66 @@
       </c>
       <c r="U16" s="5">
         <f>U15/11</f>
-        <v>0.18181818181818182</v>
+        <v>0.45454545454545453</v>
       </c>
       <c r="V16" s="5">
-        <f>V15/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="W16" s="5">
-        <f>W15/8</f>
-        <v>0.125</v>
+        <f>V15/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="W16" s="10">
+        <f>W15/6</f>
+        <v>0</v>
       </c>
       <c r="X16" s="5">
         <f>X15/11</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="Y16" s="5">
         <f>Y15/11</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="Z16" s="5">
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="Z16" s="10">
         <f>Z15/11</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="AA16" s="5">
         <f>AA15/11</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.27272727272727271</v>
       </c>
       <c r="AB16" s="5">
         <f>AB15/11</f>
-        <v>0</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AC16" s="5">
-        <f>AC15/11</f>
+        <f>AC15/3</f>
         <v>0</v>
       </c>
       <c r="AD16" s="5">
-        <f>AD15/11</f>
+        <f>AD15/2</f>
         <v>0</v>
       </c>
       <c r="AE16" s="5">
         <f>AE15/8</f>
-        <v>0</v>
-      </c>
-      <c r="AF16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AF16" s="5">
         <f>AF15/6</f>
         <v>0</v>
       </c>
       <c r="AG16" s="5">
-        <f>AG15/3</f>
-        <v>0</v>
+        <f>AG15/8</f>
+        <v>0.375</v>
       </c>
       <c r="AH16" s="5">
-        <f>AH15/2</f>
-        <v>0</v>
+        <f>AH15/5</f>
+        <v>0.6</v>
       </c>
       <c r="AI16" s="5">
-        <f>AI15/6</f>
+        <f>AI15/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="AJ16" s="5">
+        <f>AJ15/5</f>
         <v>0</v>
       </c>
     </row>
@@ -2649,45 +2670,49 @@
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <f>COUNTIF(B3:B13,3)</f>
-        <v>1</v>
-      </c>
-      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="C17" s="2">
         <f>COUNTIF(C3:C13,3)</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="3">
+        <v>6</v>
+      </c>
+      <c r="D17">
         <f>COUNTIF(D3:D13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="9">
         <f>COUNTIF(E3:E13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="F17" s="3">
+        <v>5</v>
+      </c>
+      <c r="F17" s="2">
         <f>COUNTIF(F3:F13,3)</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="3">
+        <v>5</v>
+      </c>
+      <c r="G17">
         <f>COUNTIF(G3:G13,3)</f>
-        <v>0</v>
-      </c>
-      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9">
         <f>COUNTIF(H3:H13,3)</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2">
         <f>COUNTIF(I3:I13,3)</f>
-        <v>1</v>
-      </c>
-      <c r="K17" s="9">
+        <v>3</v>
+      </c>
+      <c r="J17">
+        <f>COUNTIF(J3:J13,3)</f>
+        <v>3</v>
+      </c>
+      <c r="K17" s="2">
         <f>COUNTIF(K3:K13,3)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L17">
         <f>COUNTIF(L3:L13,3)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M17">
         <f>COUNTIF(M3:M13,3)</f>
@@ -2699,19 +2724,19 @@
       </c>
       <c r="O17">
         <f>COUNTIF(O3:O13,3)</f>
-        <v>1</v>
-      </c>
-      <c r="P17" s="3">
+        <v>2</v>
+      </c>
+      <c r="P17">
         <f>COUNTIF(P3:P13,3)</f>
-        <v>1</v>
-      </c>
-      <c r="Q17" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q17">
         <f>COUNTIF(Q3:Q13,3)</f>
-        <v>6</v>
-      </c>
-      <c r="R17" s="2">
+        <v>2</v>
+      </c>
+      <c r="R17">
         <f>COUNTIF(R3:R13,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S17">
         <f>COUNTIF(S3:S13,3)</f>
@@ -2721,132 +2746,136 @@
         <f>COUNTIF(T3:T13,3)</f>
         <v>2</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="3">
         <f>COUNTIF(U3:U13,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V17">
         <f>COUNTIF(V3:V13,3)</f>
         <v>2</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="9">
         <f>COUNTIF(W3:W13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="X17" s="2">
+        <v>1</v>
+      </c>
+      <c r="X17">
         <f>COUNTIF(X3:X13,3)</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="Y17">
         <f>COUNTIF(Y3:Y13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="9">
         <f>COUNTIF(Z3:Z13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="3">
         <f>COUNTIF(AA3:AA13,3)</f>
-        <v>0</v>
-      </c>
-      <c r="AB17" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB17">
         <f>COUNTIF(AB3:AB13,3)</f>
-        <v>6</v>
-      </c>
-      <c r="AC17" s="2">
-        <f>COUNTIF(AC3:AC13,3)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD17">
         <f>COUNTIF(AD3:AD13,3)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AE17">
         <f>COUNTIF(AE3:AE13,3)</f>
-        <v>2</v>
-      </c>
-      <c r="AF17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AF17">
         <f>COUNTIF(AF3:AF13,3)</f>
-        <v>1</v>
-      </c>
-      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="3">
+        <f>COUNTIF(AG3:AG13,3)</f>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
         <f>COUNTIF(AH3:AH13,3)</f>
         <v>0</v>
       </c>
       <c r="AI17">
         <f>COUNTIF(AI3:AI13,3)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="3">
+        <f>COUNTIF(AJ3:AJ13,3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="5">
-        <f>B17/2</f>
+        <f>B17/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="C18" s="5">
+        <f>C17/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="D18" s="5">
+        <f>D17/2</f>
         <v>0.5</v>
       </c>
-      <c r="C18" s="5">
-        <f>C17/8</f>
-        <v>0</v>
-      </c>
-      <c r="D18" s="5">
-        <f>D17/11</f>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="E18" s="5">
-        <f>E17/8</f>
+      <c r="E18" s="10">
+        <f>E17/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="F18" s="5">
+        <f>F17/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="G18" s="5">
+        <f>G17/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="H18" s="5">
+        <f>H17/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I18" s="5">
+        <f>I17/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="J18" s="5">
+        <f>J17/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="K18" s="5">
+        <f>K17/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="L18" s="5">
+        <f>L17/8</f>
         <v>0.25</v>
       </c>
-      <c r="F18" s="5">
-        <f>F17/8</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="5">
-        <f>G17/8</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="5">
-        <f>H17/8</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="10">
-        <f>I17/11</f>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="J18" s="5">
-        <f>J17/3</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="10">
-        <f>K17/11</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="L18" s="5">
-        <f>L17/11</f>
-        <v>0.36363636363636365</v>
-      </c>
       <c r="M18" s="5">
-        <f>M17/11</f>
-        <v>0.18181818181818182</v>
+        <f>M17/8</f>
+        <v>0.25</v>
       </c>
       <c r="N18" s="5">
-        <f>N17/11</f>
-        <v>0.18181818181818182</v>
+        <f>N17/8</f>
+        <v>0.25</v>
       </c>
       <c r="O18" s="5">
-        <f>O17/11</f>
-        <v>9.0909090909090912E-2</v>
+        <f>O17/8</f>
+        <v>0.25</v>
       </c>
       <c r="P18" s="5">
         <f>P17/11</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="Q18" s="5">
         <f>Q17/11</f>
-        <v>0.54545454545454541</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="R18" s="5">
         <f>R17/11</f>
-        <v>0.27272727272727271</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="S18" s="5">
         <f>S17/11</f>
@@ -2858,62 +2887,66 @@
       </c>
       <c r="U18" s="5">
         <f>U17/11</f>
-        <v>9.0909090909090912E-2</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="V18" s="5">
-        <f>V17/8</f>
-        <v>0.25</v>
-      </c>
-      <c r="W18" s="5">
-        <f>W17/8</f>
-        <v>0.25</v>
+        <f>V17/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="W18" s="10">
+        <f>W17/6</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="X18" s="5">
         <f>X17/11</f>
-        <v>0.45454545454545453</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="Y18" s="5">
         <f>Y17/11</f>
-        <v>0.18181818181818182</v>
-      </c>
-      <c r="Z18" s="5">
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z18" s="10">
         <f>Z17/11</f>
-        <v>0.18181818181818182</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AA18" s="5">
         <f>AA17/11</f>
-        <v>0</v>
+        <v>9.0909090909090912E-2</v>
       </c>
       <c r="AB18" s="5">
         <f>AB17/11</f>
-        <v>0.54545454545454541</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="5">
-        <f>AC17/11</f>
-        <v>0.27272727272727271</v>
+        <f>AC17/3</f>
+        <v>0</v>
       </c>
       <c r="AD18" s="5">
-        <f>AD17/11</f>
-        <v>0.27272727272727271</v>
+        <f>AD17/2</f>
+        <v>0</v>
       </c>
       <c r="AE18" s="5">
         <f>AE17/8</f>
-        <v>0.25</v>
-      </c>
-      <c r="AF18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="5">
         <f>AF17/6</f>
-        <v>0.16666666666666666</v>
+        <v>0</v>
       </c>
       <c r="AG18" s="5">
-        <f>AG17/3</f>
+        <f>AG17/8</f>
         <v>0</v>
       </c>
       <c r="AH18" s="5">
-        <f>AH17/2</f>
+        <f>AH17/5</f>
         <v>0</v>
       </c>
       <c r="AI18" s="5">
-        <f>AI17/6</f>
+        <f>AI17/8</f>
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="5">
+        <f>AJ17/5</f>
         <v>0</v>
       </c>
     </row>
@@ -2921,208 +2954,216 @@
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <f>COUNTIF(B3:B13,2)</f>
-        <v>0</v>
-      </c>
-      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
         <f>COUNTIF(C3:C13,2)</f>
-        <v>4</v>
-      </c>
-      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="D19">
         <f>COUNTIF(D3:D13,2)</f>
-        <v>4</v>
-      </c>
-      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="9">
         <f>COUNTIF(E3:E13,2)</f>
         <v>3</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="2">
         <f>COUNTIF(F3:F13,2)</f>
         <v>5</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19">
         <f>COUNTIF(G3:G13,2)</f>
-        <v>5</v>
-      </c>
-      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="H19" s="9">
         <f>COUNTIF(H3:H13,2)</f>
-        <v>5</v>
-      </c>
-      <c r="I19" s="9">
+        <v>1</v>
+      </c>
+      <c r="I19" s="2">
         <f>COUNTIF(I3:I13,2)</f>
+        <v>8</v>
+      </c>
+      <c r="J19">
+        <f>COUNTIF(J3:J13,2)</f>
+        <v>8</v>
+      </c>
+      <c r="K19" s="2">
+        <f>COUNTIF(K3:K13,2)</f>
         <v>6</v>
-      </c>
-      <c r="K19" s="9">
-        <f>COUNTIF(K3:K13,2)</f>
-        <v>3</v>
       </c>
       <c r="L19">
         <f>COUNTIF(L3:L13,2)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M19">
         <f>COUNTIF(M3:M13,2)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N19">
         <f>COUNTIF(N3:N13,2)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O19">
         <f>COUNTIF(O3:O13,2)</f>
+        <v>5</v>
+      </c>
+      <c r="P19">
+        <f>COUNTIF(P3:P13,2)</f>
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <f>COUNTIF(Q3:Q13,2)</f>
+        <v>6</v>
+      </c>
+      <c r="R19">
+        <f>COUNTIF(R3:R13,2)</f>
         <v>7</v>
-      </c>
-      <c r="P19" s="3">
-        <f>COUNTIF(P3:P13,2)</f>
-        <v>7</v>
-      </c>
-      <c r="Q19" s="2">
-        <f>COUNTIF(Q3:Q13,2)</f>
-        <v>3</v>
-      </c>
-      <c r="R19" s="2">
-        <f>COUNTIF(R3:R13,2)</f>
-        <v>6</v>
       </c>
       <c r="S19">
         <f>COUNTIF(S3:S13,2)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T19">
         <f>COUNTIF(T3:T13,2)</f>
         <v>7</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="3">
         <f>COUNTIF(U3:U13,2)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="V19">
         <f>COUNTIF(V3:V13,2)</f>
-        <v>5</v>
-      </c>
-      <c r="W19">
+        <v>8</v>
+      </c>
+      <c r="W19" s="9">
         <f>COUNTIF(W3:W13,2)</f>
         <v>5</v>
       </c>
-      <c r="X19" s="2">
+      <c r="X19">
         <f>COUNTIF(X3:X13,2)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Y19">
         <f>COUNTIF(Y3:Y13,2)</f>
-        <v>8</v>
-      </c>
-      <c r="Z19">
+        <v>7</v>
+      </c>
+      <c r="Z19" s="9">
         <f>COUNTIF(Z3:Z13,2)</f>
-        <v>8</v>
-      </c>
-      <c r="AA19">
+        <v>6</v>
+      </c>
+      <c r="AA19" s="3">
         <f>COUNTIF(AA3:AA13,2)</f>
+        <v>7</v>
+      </c>
+      <c r="AB19">
+        <f>COUNTIF(AB3:AB13,2)</f>
         <v>10</v>
-      </c>
-      <c r="AB19" s="2">
-        <f>COUNTIF(AB3:AB13,2)</f>
-        <v>5</v>
-      </c>
-      <c r="AC19" s="2">
-        <f>COUNTIF(AC3:AC13,2)</f>
-        <v>8</v>
       </c>
       <c r="AD19">
         <f>COUNTIF(AD3:AD13,2)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AE19">
         <f>COUNTIF(AE3:AE13,2)</f>
+        <v>4</v>
+      </c>
+      <c r="AF19">
+        <f>COUNTIF(AF3:AF13,2)</f>
         <v>6</v>
       </c>
-      <c r="AF19" s="9">
-        <f>COUNTIF(AF3:AF13,2)</f>
+      <c r="AG19" s="3">
+        <f>COUNTIF(AG3:AG13,2)</f>
         <v>5</v>
       </c>
-      <c r="AH19">
+      <c r="AH19" s="3">
         <f>COUNTIF(AH3:AH13,2)</f>
         <v>2</v>
       </c>
       <c r="AI19">
         <f>COUNTIF(AI3:AI13,2)</f>
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="AJ19" s="3">
+        <f>COUNTIF(AJ3:AJ13,2)</f>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:53" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="5">
-        <f>B19/2</f>
-        <v>0</v>
+        <f>B19/11</f>
+        <v>0.45454545454545453</v>
       </c>
       <c r="C20" s="5">
-        <f>C19/8</f>
-        <v>0.5</v>
+        <f>C19/11</f>
+        <v>0.27272727272727271</v>
       </c>
       <c r="D20" s="5">
-        <f>D19/11</f>
+        <f>D19/2</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <f>E19/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="F20" s="5">
+        <f>F19/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="G20" s="5">
+        <f>G19/11</f>
         <v>0.36363636363636365</v>
       </c>
-      <c r="E20" s="5">
-        <f>E19/8</f>
+      <c r="H20" s="5">
+        <f>H19/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I20" s="5">
+        <f>I19/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="J20" s="5">
+        <f>J19/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="K20" s="5">
+        <f>K19/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="L20" s="5">
+        <f>L19/8</f>
+        <v>0.75</v>
+      </c>
+      <c r="M20" s="5">
+        <f>M19/8</f>
         <v>0.375</v>
       </c>
-      <c r="F20" s="5">
-        <f>F19/8</f>
+      <c r="N20" s="5">
+        <f>N19/8</f>
         <v>0.625</v>
       </c>
-      <c r="G20" s="5">
-        <f>G19/8</f>
+      <c r="O20" s="5">
+        <f>O19/8</f>
         <v>0.625</v>
-      </c>
-      <c r="H20" s="5">
-        <f>H19/8</f>
-        <v>0.625</v>
-      </c>
-      <c r="I20" s="10">
-        <f>I19/11</f>
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="J20" s="5">
-        <f>J19/3</f>
-        <v>0</v>
-      </c>
-      <c r="K20" s="10">
-        <f>K19/11</f>
-        <v>0.27272727272727271</v>
-      </c>
-      <c r="L20" s="5">
-        <f>L19/11</f>
-        <v>0.36363636363636365</v>
-      </c>
-      <c r="M20" s="5">
-        <f>M19/11</f>
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="N20" s="5">
-        <f>N19/11</f>
-        <v>0.54545454545454541</v>
-      </c>
-      <c r="O20" s="5">
-        <f>O19/11</f>
-        <v>0.63636363636363635</v>
       </c>
       <c r="P20" s="5">
         <f>P19/11</f>
-        <v>0.63636363636363635</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="Q20" s="5">
         <f>Q19/11</f>
-        <v>0.27272727272727271</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="R20" s="5">
         <f>R19/11</f>
-        <v>0.54545454545454541</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="S20" s="5">
         <f>S19/11</f>
-        <v>0.63636363636363635</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="T20" s="5">
         <f>T19/11</f>
@@ -3130,62 +3171,66 @@
       </c>
       <c r="U20" s="5">
         <f>U19/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="V20" s="5">
+        <f>V19/11</f>
         <v>0.72727272727272729</v>
       </c>
-      <c r="V20" s="5">
-        <f>V19/8</f>
-        <v>0.625</v>
-      </c>
-      <c r="W20" s="5">
-        <f>W19/8</f>
-        <v>0.625</v>
+      <c r="W20" s="10">
+        <f>W19/6</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="X20" s="5">
         <f>X19/11</f>
-        <v>0.45454545454545453</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="Y20" s="5">
         <f>Y19/11</f>
-        <v>0.72727272727272729</v>
-      </c>
-      <c r="Z20" s="5">
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="Z20" s="10">
         <f>Z19/11</f>
-        <v>0.72727272727272729</v>
+        <v>0.54545454545454541</v>
       </c>
       <c r="AA20" s="5">
         <f>AA19/11</f>
-        <v>0.90909090909090906</v>
+        <v>0.63636363636363635</v>
       </c>
       <c r="AB20" s="5">
         <f>AB19/11</f>
-        <v>0.45454545454545453</v>
+        <v>0.90909090909090906</v>
       </c>
       <c r="AC20" s="5">
-        <f>AC19/11</f>
-        <v>0.72727272727272729</v>
+        <f>AC19/3</f>
+        <v>0</v>
       </c>
       <c r="AD20" s="5">
-        <f>AD19/11</f>
-        <v>0.72727272727272729</v>
+        <f>AD19/2</f>
+        <v>1</v>
       </c>
       <c r="AE20" s="5">
         <f>AE19/8</f>
-        <v>0.75</v>
-      </c>
-      <c r="AF20" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="AF20" s="5">
         <f>AF19/6</f>
-        <v>0.83333333333333337</v>
+        <v>1</v>
       </c>
       <c r="AG20" s="5">
-        <f>AG19/3</f>
-        <v>0</v>
+        <f>AG19/8</f>
+        <v>0.625</v>
       </c>
       <c r="AH20" s="5">
-        <f>AH19/2</f>
-        <v>1</v>
+        <f>AH19/5</f>
+        <v>0.4</v>
       </c>
       <c r="AI20" s="5">
-        <f>AI19/6</f>
+        <f>AI19/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="AJ20" s="5">
+        <f>AJ19/3</f>
         <v>1</v>
       </c>
     </row>
@@ -6905,8 +6950,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:AI20">
-    <sortCondition descending="1" ref="B16:AI16"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="B1:AJ20">
+    <sortCondition descending="1" ref="B18:AJ18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sound similarity fix 3
</commit_message>
<xml_diff>
--- a/Analysis/Similarity_analysis.xlsx
+++ b/Analysis/Similarity_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{634219AC-379C-4720-934C-794E39275245}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9BCDEF3B-B314-41F4-8957-93CA9ABC53E0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
   <si>
     <t>Baby_A.wav</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Test/Lures/Bubbles_B.wav</t>
+  </si>
+  <si>
+    <t>Faucet_C.wav</t>
+  </si>
+  <si>
+    <t>Footsteps_F.wav</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -685,12 +691,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -852,7 +852,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -864,8 +864,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1221,668 +1219,1022 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A580A11-5D76-4F9C-BECA-3212F55F2377}">
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="13" max="13" width="8.7265625" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="O1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="P1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L1" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="M1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="O1" t="s">
-        <v>110</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="T1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="U1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="T1" s="11" t="s">
+      <c r="W1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="Y1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="V1" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" t="s">
-        <v>97</v>
+      <c r="Z1" s="7" t="s">
+        <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="11">
-        <v>3</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>3</v>
-      </c>
-      <c r="R2">
-        <v>2</v>
-      </c>
-      <c r="S2" s="11">
-        <v>1</v>
-      </c>
-      <c r="T2" s="11">
-        <v>3</v>
-      </c>
-      <c r="U2" s="11">
-        <v>2</v>
-      </c>
-      <c r="V2">
-        <v>2</v>
-      </c>
-      <c r="W2" s="11">
-        <v>3</v>
-      </c>
-      <c r="X2">
+    <row r="2" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
+        <v>3</v>
+      </c>
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="J2" s="7">
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7">
+        <v>1</v>
+      </c>
+      <c r="M2" s="7">
+        <v>2</v>
+      </c>
+      <c r="N2" s="7">
+        <v>2</v>
+      </c>
+      <c r="O2" s="7">
+        <v>1</v>
+      </c>
+      <c r="P2" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>3</v>
+      </c>
+      <c r="R2" s="7">
+        <v>1</v>
+      </c>
+      <c r="S2" s="7">
+        <v>1</v>
+      </c>
+      <c r="T2" s="7">
+        <v>1</v>
+      </c>
+      <c r="U2" s="7">
+        <v>3</v>
+      </c>
+      <c r="V2" s="7">
+        <v>2</v>
+      </c>
+      <c r="W2" s="7">
+        <v>2</v>
+      </c>
+      <c r="X2" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>2</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3">
-        <v>3</v>
-      </c>
-      <c r="N3" s="11">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>2</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3" s="11">
-        <v>3</v>
-      </c>
-      <c r="T3" s="11">
-        <v>3</v>
-      </c>
-      <c r="U3" s="11">
-        <v>3</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3" s="11">
-        <v>2</v>
-      </c>
-      <c r="X3">
+    <row r="3" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="7">
+        <v>2</v>
+      </c>
+      <c r="C3" s="7">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2</v>
+      </c>
+      <c r="J3" s="7">
+        <v>3</v>
+      </c>
+      <c r="K3" s="7">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7">
+        <v>3</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1</v>
+      </c>
+      <c r="O3" s="7">
+        <v>2</v>
+      </c>
+      <c r="P3" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2</v>
+      </c>
+      <c r="R3" s="7">
+        <v>3</v>
+      </c>
+      <c r="S3" s="7">
+        <v>2</v>
+      </c>
+      <c r="T3" s="7">
+        <v>2</v>
+      </c>
+      <c r="U3" s="7">
+        <v>1</v>
+      </c>
+      <c r="V3" s="7">
+        <v>2</v>
+      </c>
+      <c r="W3" s="7">
+        <v>3</v>
+      </c>
+      <c r="X3" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y3" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4" s="11">
-        <v>2</v>
-      </c>
-      <c r="O4">
-        <v>2</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>2</v>
-      </c>
-      <c r="R4">
-        <v>3</v>
-      </c>
-      <c r="S4" s="11">
-        <v>3</v>
-      </c>
-      <c r="T4" s="11">
-        <v>3</v>
-      </c>
-      <c r="U4" s="11">
-        <v>2</v>
-      </c>
-      <c r="V4">
-        <v>3</v>
-      </c>
-      <c r="W4" s="11">
-        <v>2</v>
-      </c>
-      <c r="X4">
+    <row r="4" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7">
+        <v>3</v>
+      </c>
+      <c r="J4" s="7">
+        <v>2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2</v>
+      </c>
+      <c r="N4" s="7">
+        <v>2</v>
+      </c>
+      <c r="O4" s="7">
+        <v>3</v>
+      </c>
+      <c r="P4" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="7">
+        <v>2</v>
+      </c>
+      <c r="R4" s="7">
+        <v>3</v>
+      </c>
+      <c r="S4" s="7">
+        <v>2</v>
+      </c>
+      <c r="T4" s="7">
+        <v>2</v>
+      </c>
+      <c r="U4" s="7">
+        <v>2</v>
+      </c>
+      <c r="V4" s="7">
+        <v>3</v>
+      </c>
+      <c r="W4" s="7">
+        <v>2</v>
+      </c>
+      <c r="X4" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-      <c r="N5" s="11">
-        <v>2</v>
-      </c>
-      <c r="O5">
-        <v>3</v>
-      </c>
-      <c r="P5">
-        <v>2</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
-      <c r="S5" s="11">
-        <v>2</v>
-      </c>
-      <c r="T5" s="11">
-        <v>3</v>
-      </c>
-      <c r="U5" s="11">
-        <v>2</v>
-      </c>
-      <c r="V5">
-        <v>2</v>
-      </c>
-      <c r="W5" s="11">
-        <v>3</v>
-      </c>
-      <c r="X5">
+    <row r="5" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="7">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>2</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2</v>
+      </c>
+      <c r="J5" s="7">
+        <v>2</v>
+      </c>
+      <c r="K5" s="7">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7">
+        <v>2</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2</v>
+      </c>
+      <c r="N5" s="7">
+        <v>3</v>
+      </c>
+      <c r="O5" s="7">
+        <v>2</v>
+      </c>
+      <c r="P5" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>3</v>
+      </c>
+      <c r="R5" s="7">
+        <v>2</v>
+      </c>
+      <c r="S5" s="7">
+        <v>2</v>
+      </c>
+      <c r="T5" s="7">
+        <v>2</v>
+      </c>
+      <c r="U5" s="7">
+        <v>2</v>
+      </c>
+      <c r="V5" s="7">
+        <v>2</v>
+      </c>
+      <c r="W5" s="7">
+        <v>2</v>
+      </c>
+      <c r="X5" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y5" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>1</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-      <c r="M6">
-        <v>2</v>
-      </c>
-      <c r="N6" s="11">
-        <v>3</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
-        <v>2</v>
-      </c>
-      <c r="Q6">
-        <v>2</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6" s="11">
-        <v>3</v>
-      </c>
-      <c r="T6" s="11">
-        <v>2</v>
-      </c>
-      <c r="U6" s="11">
-        <v>3</v>
-      </c>
-      <c r="V6">
-        <v>2</v>
-      </c>
-      <c r="W6" s="11">
-        <v>2</v>
-      </c>
-      <c r="X6">
-        <v>2</v>
+    <row r="6" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>3</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7">
+        <v>2</v>
+      </c>
+      <c r="J6" s="7">
+        <v>2</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <v>2</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1</v>
+      </c>
+      <c r="P6" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>2</v>
+      </c>
+      <c r="R6" s="7">
+        <v>3</v>
+      </c>
+      <c r="S6" s="7">
+        <v>2</v>
+      </c>
+      <c r="T6" s="7">
+        <v>2</v>
+      </c>
+      <c r="U6" s="7">
+        <v>2</v>
+      </c>
+      <c r="V6" s="7">
+        <v>1</v>
+      </c>
+      <c r="W6" s="7">
+        <v>2</v>
+      </c>
+      <c r="X6" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y6" s="7">
+        <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="N7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="W7" s="11"/>
+    <row r="7" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="7">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="7">
+        <v>2</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>1</v>
+      </c>
+      <c r="K8" s="7">
+        <v>2</v>
+      </c>
+      <c r="L8" s="7">
+        <v>3</v>
+      </c>
+      <c r="M8" s="7">
+        <v>2</v>
+      </c>
+      <c r="N8" s="7">
+        <v>2</v>
+      </c>
+      <c r="O8" s="7">
+        <v>2</v>
+      </c>
+      <c r="P8" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>1</v>
+      </c>
+      <c r="R8" s="7">
+        <v>1</v>
+      </c>
+      <c r="S8" s="7">
+        <v>1</v>
+      </c>
+      <c r="T8" s="7">
+        <v>2</v>
+      </c>
+      <c r="U8" s="7">
+        <v>2</v>
+      </c>
+      <c r="V8" s="7">
+        <v>2</v>
+      </c>
+      <c r="W8" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <f t="shared" ref="A8:X8" si="0">COUNTIF(A2:A6,1)/5</f>
-        <v>1</v>
-      </c>
-      <c r="B8" s="4">
+    <row r="9" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7">
+        <v>1</v>
+      </c>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2</v>
+      </c>
+      <c r="J9" s="7">
+        <v>2</v>
+      </c>
+      <c r="K9" s="7">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>2</v>
+      </c>
+      <c r="M9" s="7">
+        <v>3</v>
+      </c>
+      <c r="N9" s="7">
+        <v>2</v>
+      </c>
+      <c r="O9" s="7">
+        <v>2</v>
+      </c>
+      <c r="P9" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="7">
+        <v>1</v>
+      </c>
+      <c r="R9" s="7">
+        <v>2</v>
+      </c>
+      <c r="S9" s="7">
+        <v>2</v>
+      </c>
+      <c r="T9" s="7">
+        <v>2</v>
+      </c>
+      <c r="U9" s="7">
+        <v>3</v>
+      </c>
+      <c r="V9" s="7">
+        <v>2</v>
+      </c>
+      <c r="W9" s="7">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="7">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7">
+        <v>1</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1</v>
+      </c>
+      <c r="I10" s="7">
+        <v>3</v>
+      </c>
+      <c r="J10" s="7">
+        <v>2</v>
+      </c>
+      <c r="K10" s="7">
+        <v>2</v>
+      </c>
+      <c r="L10" s="7">
+        <v>2</v>
+      </c>
+      <c r="M10" s="7">
+        <v>2</v>
+      </c>
+      <c r="N10" s="7">
+        <v>1</v>
+      </c>
+      <c r="O10" s="7">
+        <v>2</v>
+      </c>
+      <c r="P10" s="7">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="7">
+        <v>2</v>
+      </c>
+      <c r="R10" s="7">
+        <v>2</v>
+      </c>
+      <c r="S10" s="7">
+        <v>2</v>
+      </c>
+      <c r="T10" s="7">
+        <v>2</v>
+      </c>
+      <c r="U10" s="7">
+        <v>2</v>
+      </c>
+      <c r="V10" s="7">
+        <v>3</v>
+      </c>
+      <c r="W10" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A12" s="4">
+        <f>COUNTIF(A2:A10,1)/8</f>
+        <v>0.75</v>
+      </c>
+      <c r="B12" s="4">
+        <f>COUNTIF(B2:B10,1)/8</f>
+        <v>0.625</v>
+      </c>
+      <c r="C12" s="4">
+        <f>COUNTIF(C2:C6,1)/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="D12" s="4">
+        <f>COUNTIF(D2:D10,1)/8</f>
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="4">
+        <f>COUNTIF(E2:E10,1)/8</f>
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="4">
+        <f>COUNTIF(F2:F10,1)/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="G12" s="4">
+        <f>COUNTIF(G2:G10,1)/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="H12" s="4">
+        <f>COUNTIF(H2:H10,1)/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="I12" s="4">
+        <f>COUNTIF(I2:I10,1)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" ref="J12:R12" si="0">COUNTIF(J2:J10,1)/8</f>
+        <v>0.25</v>
+      </c>
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="C8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="L12" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="M12" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="E8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N12" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="F8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="O12" s="4">
         <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="G8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="P12" s="4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="H8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="Q12" s="4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="I8" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="R12" s="4">
         <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="J8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="K8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="L8" s="4">
-        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="S12" s="4">
+        <f>COUNTIF(S2:S6,1)/5</f>
         <v>0.2</v>
       </c>
-      <c r="M8" s="4">
-        <f t="shared" si="0"/>
+      <c r="T12" s="4">
+        <f t="shared" ref="T12:Y12" si="1">COUNTIF(T2:T10,1)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="W12" s="4">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="X12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Z12" s="4">
+        <f>COUNTIF(Z2:Z10,1)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A13" s="4">
+        <f>COUNTIF(A2:A10,3)/8</f>
+        <v>0</v>
+      </c>
+      <c r="B13" s="4">
+        <f>COUNTIF(B2:B10,3)/8</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="4">
+        <f>COUNTIF(C2:C6,3)/5</f>
         <v>0.2</v>
       </c>
-      <c r="N8" s="12">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="O8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="P8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="Q8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="R8" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="S8" s="12">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="T8" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U8" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W8" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="X8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+      <c r="D13" s="4">
+        <f>COUNTIF(D2:D10,3)/8</f>
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="4">
+        <f>COUNTIF(E2:E10,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="F13" s="4">
+        <f>COUNTIF(F2:F10,3)/8</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="4">
+        <f>COUNTIF(G2:G10,3)/8</f>
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="4">
+        <f>COUNTIF(H2:H10,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="I13" s="4">
+        <f>COUNTIF(I2:I10,3)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" ref="J13:R13" si="2">COUNTIF(J2:J10,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="K13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="M13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="N13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="O13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.125</v>
+      </c>
+      <c r="P13" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="R13" s="4">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="S13" s="4">
+        <f>COUNTIF(S2:S6,3)/5</f>
+        <v>0</v>
+      </c>
+      <c r="T13" s="4">
+        <f t="shared" ref="T13:Y13" si="3">COUNTIF(T2:T10,3)/8</f>
+        <v>0</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="W13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.125</v>
+      </c>
+      <c r="X13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y13" s="4">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="Z13" s="4">
+        <f>COUNTIF(Z2:Z10,3)/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <f t="shared" ref="A9:X9" si="1">COUNTIF(A2:A6,3)/5</f>
-        <v>0</v>
-      </c>
-      <c r="B9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="C9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="I9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="K9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="N9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="O9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="P9" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="R9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="S9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.6</v>
-      </c>
-      <c r="T9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
-      </c>
-      <c r="U9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="V9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
-      </c>
-      <c r="W9" s="12">
-        <f t="shared" si="1"/>
-        <v>0.4</v>
-      </c>
-      <c r="X9" s="4">
-        <f t="shared" si="1"/>
-        <v>0.2</v>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A14" s="4">
+        <f>COUNTIF(A2:A10,2)/8</f>
+        <v>0.25</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" ref="B14:Z14" si="4">COUNTIF(B2:B10,2)/8</f>
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="M14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="N14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="O14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="P14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.5</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="T14" s="4">
+        <f>COUNTIF(T2:T10,2)/8</f>
+        <v>0.875</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.625</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.75</v>
+      </c>
+      <c r="X14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="Y14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.375</v>
+      </c>
+      <c r="Z14" s="4">
+        <f t="shared" si="4"/>
+        <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="N11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="W11" s="2"/>
+    <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="Z15" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:BD13">
+    <sortCondition descending="1" ref="A12:BD12"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Sound similarity change 4
</commit_message>
<xml_diff>
--- a/Analysis/Similarity_analysis.xlsx
+++ b/Analysis/Similarity_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwoca-my.sharepoint.com/personal/swan689_uwo_ca/Documents/Desktop/Project BL/Guess The Sound/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="64" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9BCDEF3B-B314-41F4-8957-93CA9ABC53E0}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="13_ncr:40009_{2C9B549A-3F7C-4296-A8F6-66C1DA968382}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{832542FF-8257-4497-B943-F1909E742908}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="118">
   <si>
     <t>Baby_A.wav</t>
   </si>
@@ -363,6 +363,18 @@
   </si>
   <si>
     <t>Footsteps_F.wav</t>
+  </si>
+  <si>
+    <t>Growl_H.wav</t>
+  </si>
+  <si>
+    <t>Laugh_F.wav</t>
+  </si>
+  <si>
+    <t>Snore_E.wav</t>
+  </si>
+  <si>
+    <t>Phone</t>
   </si>
 </sst>
 </file>
@@ -505,7 +517,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -691,6 +703,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -852,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -864,6 +894,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1219,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A580A11-5D76-4F9C-BECA-3212F55F2377}">
-  <dimension ref="A1:Z15"/>
+  <dimension ref="A1:AD21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1230,7 +1263,7 @@
     <col min="13" max="13" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
@@ -1238,79 +1271,91 @@
         <v>109</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>105</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>70</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>104</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="N1" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="O1" t="s">
+        <v>114</v>
+      </c>
+      <c r="P1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="V1" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="X1" s="7" t="s">
+      <c r="AA1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="AB1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="Z1" s="7" t="s">
-        <v>113</v>
+      <c r="AC1" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1323,41 +1368,32 @@
       <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
-        <v>1</v>
-      </c>
       <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H2" s="7">
+        <v>3</v>
+      </c>
+      <c r="I2" s="7">
         <v>2</v>
       </c>
       <c r="J2" s="7">
         <v>1</v>
       </c>
       <c r="K2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L2" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M2" s="7">
         <v>2</v>
       </c>
-      <c r="N2" s="7">
-        <v>2</v>
-      </c>
-      <c r="O2" s="7">
-        <v>1</v>
-      </c>
-      <c r="P2" s="7">
-        <v>1</v>
-      </c>
       <c r="Q2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R2" s="7">
         <v>1</v>
@@ -1366,25 +1402,34 @@
         <v>1</v>
       </c>
       <c r="T2" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U2" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="V2" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W2" s="7">
         <v>2</v>
       </c>
       <c r="X2" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y2" s="7">
         <v>2</v>
       </c>
+      <c r="Z2" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="3" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -1397,68 +1442,68 @@
       <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="7">
-        <v>2</v>
-      </c>
       <c r="F3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="7">
         <v>2</v>
       </c>
+      <c r="I3" s="7">
+        <v>2</v>
+      </c>
       <c r="J3" s="7">
         <v>3</v>
       </c>
       <c r="K3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M3" s="7">
         <v>1</v>
       </c>
-      <c r="N3" s="7">
-        <v>1</v>
-      </c>
-      <c r="O3" s="7">
-        <v>2</v>
-      </c>
-      <c r="P3" s="7">
-        <v>2</v>
-      </c>
       <c r="Q3" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S3" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T3" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U3" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V3" s="7">
         <v>2</v>
       </c>
       <c r="W3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="X3" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y3" s="7">
         <v>3</v>
       </c>
+      <c r="Z3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB3" s="7">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -1471,59 +1516,50 @@
       <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
       <c r="F4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="7">
         <v>2</v>
       </c>
       <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="I4" s="7">
         <v>3</v>
       </c>
       <c r="J4" s="7">
         <v>2</v>
       </c>
       <c r="K4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="7">
         <v>2</v>
       </c>
-      <c r="N4" s="7">
-        <v>2</v>
-      </c>
-      <c r="O4" s="7">
-        <v>3</v>
-      </c>
-      <c r="P4" s="7">
-        <v>2</v>
-      </c>
       <c r="Q4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S4" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T4" s="7">
         <v>2</v>
       </c>
       <c r="U4" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V4" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W4" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X4" s="7">
         <v>3</v>
@@ -1531,8 +1567,17 @@
       <c r="Y4" s="7">
         <v>2</v>
       </c>
+      <c r="Z4" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>1</v>
       </c>
@@ -1540,21 +1585,21 @@
         <v>2</v>
       </c>
       <c r="C5" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
       <c r="F5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="7">
+        <v>3</v>
+      </c>
+      <c r="I5" s="7">
         <v>2</v>
       </c>
       <c r="J5" s="7">
@@ -1569,17 +1614,8 @@
       <c r="M5" s="7">
         <v>2</v>
       </c>
-      <c r="N5" s="7">
-        <v>3</v>
-      </c>
-      <c r="O5" s="7">
-        <v>2</v>
-      </c>
-      <c r="P5" s="7">
-        <v>1</v>
-      </c>
       <c r="Q5" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R5" s="7">
         <v>2</v>
@@ -1588,7 +1624,7 @@
         <v>2</v>
       </c>
       <c r="T5" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U5" s="7">
         <v>2</v>
@@ -1600,13 +1636,22 @@
         <v>2</v>
       </c>
       <c r="X5" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="7">
         <v>2</v>
       </c>
+      <c r="Z5" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>3</v>
+      </c>
+      <c r="AB5" s="7">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>1</v>
       </c>
@@ -1614,23 +1659,23 @@
         <v>1</v>
       </c>
       <c r="C6" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="E6" s="7">
-        <v>1</v>
-      </c>
       <c r="F6" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="7">
         <v>2</v>
       </c>
+      <c r="I6" s="7">
+        <v>2</v>
+      </c>
       <c r="J6" s="7">
         <v>2</v>
       </c>
@@ -1638,50 +1683,50 @@
         <v>1</v>
       </c>
       <c r="L6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="7">
         <v>1</v>
       </c>
-      <c r="N6" s="7">
-        <v>2</v>
-      </c>
-      <c r="O6" s="7">
-        <v>1</v>
-      </c>
-      <c r="P6" s="7">
-        <v>2</v>
-      </c>
       <c r="Q6" s="7">
         <v>2</v>
       </c>
       <c r="R6" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S6" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T6" s="7">
         <v>2</v>
       </c>
       <c r="U6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V6" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X6" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y6" s="7">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="7">
+        <v>2</v>
+      </c>
+      <c r="AB6" s="7">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>2</v>
       </c>
@@ -1689,16 +1734,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D8" s="7">
         <v>2</v>
       </c>
       <c r="E8" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="7">
         <v>2</v>
@@ -1716,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="L8" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M8" s="7">
         <v>2</v>
@@ -1724,17 +1769,11 @@
       <c r="N8" s="7">
         <v>2</v>
       </c>
-      <c r="O8" s="7">
-        <v>2</v>
-      </c>
-      <c r="P8" s="7">
-        <v>2</v>
-      </c>
       <c r="Q8" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R8" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" s="7">
         <v>1</v>
@@ -1746,16 +1785,22 @@
         <v>2</v>
       </c>
       <c r="V8" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W8" s="7">
         <v>2</v>
       </c>
+      <c r="X8" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>2</v>
+      </c>
       <c r="Z8" s="7">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>1</v>
       </c>
@@ -1763,25 +1808,25 @@
         <v>2</v>
       </c>
       <c r="C9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9" s="7">
         <v>3</v>
       </c>
       <c r="E9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
       </c>
       <c r="G9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H9" s="7">
         <v>1</v>
       </c>
       <c r="I9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="7">
         <v>2</v>
@@ -1790,7 +1835,7 @@
         <v>2</v>
       </c>
       <c r="L9" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M9" s="7">
         <v>3</v>
@@ -1798,14 +1843,8 @@
       <c r="N9" s="7">
         <v>2</v>
       </c>
-      <c r="O9" s="7">
-        <v>2</v>
-      </c>
-      <c r="P9" s="7">
-        <v>2</v>
-      </c>
       <c r="Q9" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="7">
         <v>2</v>
@@ -1817,19 +1856,25 @@
         <v>2</v>
       </c>
       <c r="U9" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V9" s="7">
         <v>2</v>
       </c>
       <c r="W9" s="7">
+        <v>2</v>
+      </c>
+      <c r="X9" s="7">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="7">
         <v>1</v>
       </c>
       <c r="Z9" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>2</v>
       </c>
@@ -1843,19 +1888,19 @@
         <v>1</v>
       </c>
       <c r="E10" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" s="7">
         <v>2</v>
       </c>
       <c r="G10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J10" s="7">
         <v>2</v>
@@ -1864,19 +1909,13 @@
         <v>2</v>
       </c>
       <c r="L10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10" s="7">
         <v>2</v>
       </c>
       <c r="N10" s="7">
-        <v>1</v>
-      </c>
-      <c r="O10" s="7">
-        <v>2</v>
-      </c>
-      <c r="P10" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q10" s="7">
         <v>2</v>
@@ -1888,352 +1927,645 @@
         <v>2</v>
       </c>
       <c r="T10" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U10" s="7">
         <v>2</v>
       </c>
       <c r="V10" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W10" s="7">
         <v>2</v>
       </c>
+      <c r="X10" s="7">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="7">
+        <v>2</v>
+      </c>
       <c r="Z10" s="7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <f>COUNTIF(A2:A10,1)/8</f>
-        <v>0.75</v>
-      </c>
-      <c r="B12" s="4">
-        <f>COUNTIF(B2:B10,1)/8</f>
-        <v>0.625</v>
-      </c>
-      <c r="C12" s="4">
-        <f>COUNTIF(C2:C6,1)/5</f>
-        <v>0.6</v>
-      </c>
-      <c r="D12" s="4">
-        <f>COUNTIF(D2:D10,1)/8</f>
+    <row r="11" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>3</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>3</v>
+      </c>
+      <c r="W12">
+        <v>3</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="AC12">
+        <v>3</v>
+      </c>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13">
+        <v>2</v>
+      </c>
+      <c r="V13">
+        <v>2</v>
+      </c>
+      <c r="W13">
+        <v>2</v>
+      </c>
+      <c r="X13">
+        <v>3</v>
+      </c>
+      <c r="Y13">
+        <v>2</v>
+      </c>
+      <c r="AC13">
+        <v>2</v>
+      </c>
+      <c r="AD13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>3</v>
+      </c>
+      <c r="V14">
+        <v>2</v>
+      </c>
+      <c r="W14">
+        <v>3</v>
+      </c>
+      <c r="X14">
+        <v>3</v>
+      </c>
+      <c r="Y14">
+        <v>2</v>
+      </c>
+      <c r="AC14">
+        <v>3</v>
+      </c>
+      <c r="AD14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <f>COUNTIF(A2:A14,1)/11</f>
+        <v>0.81818181818181823</v>
+      </c>
+      <c r="B16" s="4">
+        <f>COUNTIF(B2:B14,1)/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="C16" s="4">
+        <f>COUNTIF(C2:C14,1)/11</f>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="D16" s="4">
+        <f>COUNTIF(D2:D14,1)/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="E16" s="4">
+        <f>COUNTIF(E2:E14,1)/6</f>
         <v>0.5</v>
       </c>
-      <c r="E12" s="4">
-        <f>COUNTIF(E2:E10,1)/8</f>
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="4">
-        <f>COUNTIF(F2:F10,1)/8</f>
+      <c r="F16" s="4">
+        <f>COUNTIF(F2:F14,1)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="G16" s="4">
+        <f>COUNTIF(G2:G14,1)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="H16" s="4">
+        <f>COUNTIF(H2:H14,1)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="I16" s="4">
+        <f>COUNTIF(I2:I14,1)/8</f>
         <v>0.375</v>
       </c>
-      <c r="G12" s="4">
-        <f>COUNTIF(G2:G10,1)/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="H12" s="4">
-        <f>COUNTIF(H2:H10,1)/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="I12" s="4">
-        <f>COUNTIF(I2:I10,1)/3</f>
+      <c r="J16" s="4">
+        <f>COUNTIF(J2:J14,1)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="K16" s="4">
+        <f>COUNTIF(K2:K14,1)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="L16" s="4">
+        <f>COUNTIF(L2:L14,1)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="M16" s="4">
+        <f>COUNTIF(M2:M14,1)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="N16" s="4">
+        <f>COUNTIF(N2:N14,3)/6</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="J12" s="4">
-        <f t="shared" ref="J12:R12" si="0">COUNTIF(J2:J10,1)/8</f>
+      <c r="O16" s="4">
+        <f>COUNTIF(O2:O14,1)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P16" s="4">
+        <f>COUNTIF(P2:P14,1)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="Q16" s="4">
+        <f>COUNTIF(Q2:Q14,1)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="R16" s="4">
+        <f>COUNTIF(R2:R14,1)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="S16" s="4">
+        <f>COUNTIF(S2:S14,1)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="T16" s="4">
+        <f>COUNTIF(T2:T14,1)/8</f>
         <v>0.25</v>
       </c>
-      <c r="K12" s="4">
-        <f t="shared" si="0"/>
+      <c r="U16" s="4">
+        <f>COUNTIF(U2:U14,1)/8</f>
         <v>0.25</v>
       </c>
-      <c r="L12" s="4">
-        <f t="shared" si="0"/>
+      <c r="V16" s="4">
+        <f>COUNTIF(V2:V14,1)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="W16" s="4">
+        <f>COUNTIF(W2:W14,1)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="X16" s="4">
+        <f>COUNTIF(X2:X14,1)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="Y16" s="4">
+        <f>COUNTIF(Y2:Y14,1)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="Z16" s="4">
+        <f>COUNTIF(Z2:Z14,1)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="AA16" s="4">
+        <f>COUNTIF(AA2:AA14,1)/5</f>
+        <v>0</v>
+      </c>
+      <c r="AB16" s="4">
+        <f>COUNTIF(AB2:AB14,1)/5</f>
+        <v>0</v>
+      </c>
+      <c r="AC16" s="4">
+        <f>COUNTIF(AC2:AC14,1)/3</f>
+        <v>0</v>
+      </c>
+      <c r="AD16" s="4">
+        <f>COUNTIF(AD2:AD14,1)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <f>COUNTIF(A2:A14,3)/11</f>
+        <v>0</v>
+      </c>
+      <c r="B17" s="4">
+        <f>COUNTIF(B2:B14,3)/11</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="4">
+        <f>COUNTIF(C2:C14,3)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="D17" s="4">
+        <f>COUNTIF(D2:D14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="E17" s="4">
+        <f>COUNTIF(E2:E14,3)/6</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="F17" s="4">
+        <f>COUNTIF(F2:F14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="G17" s="4">
+        <f>COUNTIF(G2:G14,3)/11</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="4">
+        <f>COUNTIF(H2:H14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="I17" s="4">
+        <f>COUNTIF(I2:I14,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="J17" s="4">
+        <f>COUNTIF(J2:J14,3)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="K17" s="4">
+        <f>COUNTIF(K2:K14,3)/11</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <f>COUNTIF(L2:L14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="M17" s="4">
+        <f>COUNTIF(M2:M14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="N17" s="4">
+        <f>COUNTIF(N3:N15,1)/6</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="O17" s="4">
+        <f>COUNTIF(O2:O14,3)/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="P17" s="4">
+        <f>COUNTIF(P2:P14,3)/3</f>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="4">
+        <f>COUNTIF(Q2:Q14,3)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="R17" s="4">
+        <f>COUNTIF(R2:R14,3)/11</f>
+        <v>0</v>
+      </c>
+      <c r="S17" s="4">
+        <f>COUNTIF(S2:S14,3)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="T17" s="4">
+        <f>COUNTIF(T2:T14,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="U17" s="4">
+        <f>COUNTIF(U2:U14,3)/8</f>
+        <v>0.125</v>
+      </c>
+      <c r="V17" s="4">
+        <f>COUNTIF(V2:V14,3)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="W17" s="4">
+        <f>COUNTIF(W2:W14,3)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="X17" s="4">
+        <f>COUNTIF(X2:X14,3)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="Y17" s="4">
+        <f>COUNTIF(Y2:Y14,3)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Z17" s="4">
+        <f>COUNTIF(Z2:Z14,3)/8</f>
         <v>0.25</v>
       </c>
-      <c r="M12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="N12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="O12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="P12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="Q12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="R12" s="4">
-        <f t="shared" si="0"/>
-        <v>0.25</v>
-      </c>
-      <c r="S12" s="4">
-        <f>COUNTIF(S2:S6,1)/5</f>
-        <v>0.2</v>
-      </c>
-      <c r="T12" s="4">
-        <f t="shared" ref="T12:Y12" si="1">COUNTIF(T2:T10,1)/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="U12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="V12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="W12" s="4">
-        <f t="shared" si="1"/>
-        <v>0.125</v>
-      </c>
-      <c r="X12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Y12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Z12" s="4">
-        <f>COUNTIF(Z2:Z10,1)/3</f>
-        <v>0</v>
+      <c r="AA17" s="4">
+        <f>COUNTIF(AA2:AA14,3)/5</f>
+        <v>0.8</v>
+      </c>
+      <c r="AB17" s="4">
+        <f>COUNTIF(AB2:AB14,3)/5</f>
+        <v>0.4</v>
+      </c>
+      <c r="AC17" s="4">
+        <f>COUNTIF(AC2:AC14,3)/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="AD17" s="4">
+        <f>COUNTIF(AD2:AD14,3)/3</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <f>COUNTIF(A2:A10,3)/8</f>
-        <v>0</v>
-      </c>
-      <c r="B13" s="4">
-        <f>COUNTIF(B2:B10,3)/8</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <f>COUNTIF(C2:C6,3)/5</f>
-        <v>0.2</v>
-      </c>
-      <c r="D13" s="4">
-        <f>COUNTIF(D2:D10,3)/8</f>
-        <v>0.25</v>
-      </c>
-      <c r="E13" s="4">
-        <f>COUNTIF(E2:E10,3)/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="F13" s="4">
-        <f>COUNTIF(F2:F10,3)/8</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <f>COUNTIF(G2:G10,3)/8</f>
-        <v>0.25</v>
-      </c>
-      <c r="H13" s="4">
-        <f>COUNTIF(H2:H10,3)/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="I13" s="4">
-        <f>COUNTIF(I2:I10,3)/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="J13" s="4">
-        <f t="shared" ref="J13:R13" si="2">COUNTIF(J2:J10,3)/8</f>
-        <v>0.125</v>
-      </c>
-      <c r="K13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="M13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="N13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="O13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.125</v>
-      </c>
-      <c r="P13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.25</v>
-      </c>
-      <c r="R13" s="4">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
-      </c>
-      <c r="S13" s="4">
-        <f>COUNTIF(S2:S6,3)/5</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
-        <f t="shared" ref="T13:Y13" si="3">COUNTIF(T2:T10,3)/8</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="V13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="W13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.125</v>
-      </c>
-      <c r="X13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.5</v>
-      </c>
-      <c r="Y13" s="4">
-        <f t="shared" si="3"/>
-        <v>0.25</v>
-      </c>
-      <c r="Z13" s="4">
-        <f>COUNTIF(Z2:Z10,3)/3</f>
-        <v>0.33333333333333331</v>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <f>COUNTIF(A2:A14,2)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="B18" s="4">
+        <f>COUNTIF(B2:B14,2)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="C18" s="4">
+        <f>COUNTIF(C2:C14,2)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="D18" s="4">
+        <f>COUNTIF(D2:D14,2)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="E18" s="4">
+        <f>COUNTIF(E2:E14,2)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="F18" s="4">
+        <f>COUNTIF(F2:F14,2)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="G18" s="4">
+        <f>COUNTIF(G2:G14,2)/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="H18" s="4">
+        <f>COUNTIF(H2:H14,2)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="I18" s="4">
+        <f>COUNTIF(I2:I14,2)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="J18" s="4">
+        <f>COUNTIF(J2:J14,2)/11</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="K18" s="4">
+        <f>COUNTIF(K2:K14,2)/11</f>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="L18" s="4">
+        <f>COUNTIF(L2:L14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="M18" s="4">
+        <f>COUNTIF(M2:M14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="N18" s="4">
+        <f>COUNTIF(N2:N14,2)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="O18" s="4">
+        <f>COUNTIF(O2:O14,2)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="P18" s="4">
+        <f>COUNTIF(P2:P14,2)/11</f>
+        <v>0.18181818181818182</v>
+      </c>
+      <c r="Q18" s="4">
+        <f>COUNTIF(Q2:Q14,2)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="R18" s="4">
+        <f>COUNTIF(R2:R14,2)/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="S18" s="4">
+        <f>COUNTIF(S2:S14,2)/11</f>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="T18" s="4">
+        <f>COUNTIF(T2:T14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="U18" s="4">
+        <f>COUNTIF(U2:U14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="V18" s="4">
+        <f>COUNTIF(V2:V14,2)/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="W18" s="4">
+        <f>COUNTIF(W2:W14,2)/11</f>
+        <v>0.63636363636363635</v>
+      </c>
+      <c r="X18" s="4">
+        <f>COUNTIF(X2:X14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="Y18" s="4">
+        <f>COUNTIF(Y2:Y14,2)/11</f>
+        <v>0.72727272727272729</v>
+      </c>
+      <c r="Z18" s="4">
+        <f>COUNTIF(Z2:Z14,2)/11</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="AA18" s="4">
+        <f>COUNTIF(AA2:AA14,2)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AB18" s="4">
+        <f>COUNTIF(AB2:AB14,2)/11</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="AC18" s="4">
+        <f>COUNTIF(AC2:AC14,2)/11</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="AD18" s="4">
+        <f>COUNTIF(AD2:AD14,2)/11</f>
+        <v>0.18181818181818182</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <f>COUNTIF(A2:A10,2)/8</f>
-        <v>0.25</v>
-      </c>
-      <c r="B14" s="4">
-        <f t="shared" ref="B14:Z14" si="4">COUNTIF(B2:B10,2)/8</f>
-        <v>0.375</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="H14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="I14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.125</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="K14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="M14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="N14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="O14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="P14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="Q14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-      <c r="R14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="S14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="T14" s="4">
-        <f>COUNTIF(T2:T10,2)/8</f>
-        <v>0.875</v>
-      </c>
-      <c r="U14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="V14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.625</v>
-      </c>
-      <c r="W14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.75</v>
-      </c>
-      <c r="X14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.125</v>
-      </c>
-      <c r="Y14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.375</v>
-      </c>
-      <c r="Z14" s="4">
-        <f t="shared" si="4"/>
-        <v>0.25</v>
-      </c>
+    <row r="19" spans="1:30" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
     </row>
-    <row r="15" spans="1:26" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="Z15" s="2"/>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.35">
+      <c r="J21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:BD13">
-    <sortCondition descending="1" ref="A12:BD12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:BH19">
+    <sortCondition descending="1" ref="A16:BH16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>